<commit_message>
Fix #791: Add import support for select_multiple attribute types
</commit_message>
<xml_diff>
--- a/cadasta/organization/tests/files/uttaran_test.xlsx
+++ b/cadasta/organization/tests/files/uttaran_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="966" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="404" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="650">
   <si>
     <t>type</t>
   </si>
@@ -178,7 +178,7 @@
     <t>audio_hh</t>
   </si>
   <si>
-    <t>অডিও নিন </t>
+    <t>অডিও নিন</t>
   </si>
   <si>
     <t>Record audio</t>
@@ -301,7 +301,7 @@
     <t>educational_qualification</t>
   </si>
   <si>
-    <t>শিক্ষাগত যোগ্যতা </t>
+    <t>শিক্ষাগত যোগ্যতা</t>
   </si>
   <si>
     <t>Eduational level</t>
@@ -412,7 +412,7 @@
     <t>How the tribal adquired the land?</t>
   </si>
   <si>
-    <t>generations </t>
+    <t>generations</t>
   </si>
   <si>
     <t>${class_HH}='tribal'</t>
@@ -568,9 +568,6 @@
     <t>Is there any boundary conflict?</t>
   </si>
   <si>
-    <t> </t>
-  </si>
-  <si>
     <t>others_conflict</t>
   </si>
   <si>
@@ -631,7 +628,7 @@
     <t>nid_number</t>
   </si>
   <si>
-    <t>আপনার ভোটার/ জন্ম নিবন্ধন নং বলুন </t>
+    <t>আপনার ভোটার/ জন্ম নিবন্ধন নং বলুন</t>
   </si>
   <si>
     <t>National ID number</t>
@@ -646,6 +643,15 @@
     <t>Name of data collector</t>
   </si>
   <si>
+    <t>select_multiple location_problems</t>
+  </si>
+  <si>
+    <t>location_problems</t>
+  </si>
+  <si>
+    <t>Location Problems</t>
+  </si>
+  <si>
     <t>tenure_relationship_attributes</t>
   </si>
   <si>
@@ -682,7 +688,7 @@
     <t>Drawing coordinates on a map</t>
   </si>
   <si>
-    <t>Walking around the boundaries </t>
+    <t>Walking around the boundaries</t>
   </si>
   <si>
     <t>land_type</t>
@@ -835,7 +841,7 @@
     <t>occupation</t>
   </si>
   <si>
-    <t>ব্যবসায়ী </t>
+    <t>ব্যবসায়ী</t>
   </si>
   <si>
     <t>farmer</t>
@@ -850,7 +856,7 @@
     <t>দিন মজুর</t>
   </si>
   <si>
-    <t>doctor </t>
+    <t>doctor</t>
   </si>
   <si>
     <t>ডাক্তার</t>
@@ -865,13 +871,13 @@
     <t>housewife</t>
   </si>
   <si>
-    <t>গৃহিনী </t>
-  </si>
-  <si>
-    <t>vandriver </t>
-  </si>
-  <si>
-    <t>ভ্যান চালক </t>
+    <t>গৃহিনী</t>
+  </si>
+  <si>
+    <t>vandriver</t>
+  </si>
+  <si>
+    <t>ভ্যান চালক</t>
   </si>
   <si>
     <t>rickshaw_puller</t>
@@ -880,10 +886,10 @@
     <t>রিক্সা চালক</t>
   </si>
   <si>
-    <t>teacher </t>
-  </si>
-  <si>
-    <t>শিক্ষক/ শিক্ষিকা </t>
+    <t>teacher</t>
+  </si>
+  <si>
+    <t>শিক্ষক/ শিক্ষিকা</t>
   </si>
   <si>
     <t>service</t>
@@ -895,7 +901,7 @@
     <t>local_representative</t>
   </si>
   <si>
-    <t>স্থানীয় জনপ্রতিনিধি </t>
+    <t>স্থানীয় জনপ্রতিনিধি</t>
   </si>
   <si>
     <t>student</t>
@@ -907,7 +913,7 @@
     <t>unemployed</t>
   </si>
   <si>
-    <t>বেকার </t>
+    <t>বেকার</t>
   </si>
   <si>
     <t>others</t>
@@ -949,7 +955,7 @@
     <t>নিরক্ষর</t>
   </si>
   <si>
-    <t>signature </t>
+    <t>signature</t>
   </si>
   <si>
     <t>স্বাক্ষরঞ্জান</t>
@@ -961,7 +967,7 @@
     <t>অক্ষরঞ্জান</t>
   </si>
   <si>
-    <t>educated </t>
+    <t>educated</t>
   </si>
   <si>
     <t>শিক্ষিত</t>
@@ -1093,6 +1099,36 @@
     <t>অকৃষি</t>
   </si>
   <si>
+    <t>risk_of_eviction</t>
+  </si>
+  <si>
+    <t>Risk of Eviction</t>
+  </si>
+  <si>
+    <t>conflict</t>
+  </si>
+  <si>
+    <t>Conflict</t>
+  </si>
+  <si>
+    <t>incomplete_rights_documents</t>
+  </si>
+  <si>
+    <t>Incomplete Rights Documents</t>
+  </si>
+  <si>
+    <t>lack_of_rights_documents</t>
+  </si>
+  <si>
+    <t>Lack of Rights Documents</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
     <t>upazilla</t>
   </si>
   <si>
@@ -1153,7 +1189,7 @@
     <t>kolaboh</t>
   </si>
   <si>
-    <t>কলাবহ </t>
+    <t>কলাবহ</t>
   </si>
   <si>
     <t>kochgor</t>
@@ -1345,13 +1381,13 @@
     <t>digarbari</t>
   </si>
   <si>
-    <t>দিগারবাড়ী </t>
+    <t>দিগারবাড়ী</t>
   </si>
   <si>
     <t>doherpar</t>
   </si>
   <si>
-    <t>দহেরপাড় </t>
+    <t>দহেরপাড়</t>
   </si>
   <si>
     <t>nashirpur</t>
@@ -1684,7 +1720,7 @@
     <t>bidrika</t>
   </si>
   <si>
-    <t>বিদি্রিকা </t>
+    <t>বিদি্রিকা</t>
   </si>
   <si>
     <t>bimpara</t>
@@ -1726,7 +1762,7 @@
     <t>shihalai</t>
   </si>
   <si>
-    <t>শিহালাই </t>
+    <t>শিহালাই</t>
   </si>
   <si>
     <t>shakoua</t>
@@ -1756,7 +1792,7 @@
     <t>sinduri</t>
   </si>
   <si>
-    <t>সিন্দুরী </t>
+    <t>সিন্দুরী</t>
   </si>
   <si>
     <t>mouza_amtali</t>
@@ -2495,12 +2531,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z65536"/>
+  <dimension ref="A1:Z79"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A72" activeCellId="0" sqref="72:77"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="F71" activeCellId="0" sqref="F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4726,9 +4762,7 @@
       <c r="I62" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="J62" s="43" t="s">
-        <v>183</v>
-      </c>
+      <c r="J62" s="43"/>
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
       <c r="M62" s="2"/>
@@ -4751,13 +4785,13 @@
         <v>22</v>
       </c>
       <c r="B63" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="C63" s="37" t="s">
         <v>184</v>
       </c>
-      <c r="C63" s="37" t="s">
+      <c r="D63" s="38" t="s">
         <v>185</v>
-      </c>
-      <c r="D63" s="38" t="s">
-        <v>186</v>
       </c>
       <c r="E63" s="41"/>
       <c r="F63" s="41"/>
@@ -4787,13 +4821,13 @@
         <v>104</v>
       </c>
       <c r="B64" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="C64" s="37" t="s">
         <v>187</v>
       </c>
-      <c r="C64" s="37" t="s">
+      <c r="D64" s="38" t="s">
         <v>188</v>
-      </c>
-      <c r="D64" s="38" t="s">
-        <v>189</v>
       </c>
       <c r="E64" s="41"/>
       <c r="F64" s="41"/>
@@ -4822,26 +4856,26 @@
     </row>
     <row r="65" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="31" t="s">
+        <v>189</v>
+      </c>
+      <c r="B65" s="31" t="s">
         <v>190</v>
       </c>
-      <c r="B65" s="31" t="s">
+      <c r="C65" s="37" t="s">
         <v>191</v>
       </c>
-      <c r="C65" s="37" t="s">
+      <c r="D65" s="38" t="s">
         <v>192</v>
-      </c>
-      <c r="D65" s="38" t="s">
-        <v>193</v>
       </c>
       <c r="E65" s="41"/>
       <c r="F65" s="41"/>
       <c r="G65" s="41"/>
       <c r="H65" s="41"/>
       <c r="I65" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="J65" s="25" t="s">
         <v>194</v>
-      </c>
-      <c r="J65" s="25" t="s">
-        <v>195</v>
       </c>
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
@@ -4865,13 +4899,13 @@
         <v>104</v>
       </c>
       <c r="B66" s="31" t="s">
+        <v>195</v>
+      </c>
+      <c r="C66" s="37" t="s">
         <v>196</v>
       </c>
-      <c r="C66" s="37" t="s">
+      <c r="D66" s="38" t="s">
         <v>197</v>
-      </c>
-      <c r="D66" s="38" t="s">
-        <v>198</v>
       </c>
       <c r="E66" s="41"/>
       <c r="F66" s="41"/>
@@ -4903,13 +4937,13 @@
         <v>22</v>
       </c>
       <c r="B67" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="C67" s="37" t="s">
         <v>199</v>
       </c>
-      <c r="C67" s="37" t="s">
+      <c r="D67" s="38" t="s">
         <v>200</v>
-      </c>
-      <c r="D67" s="38" t="s">
-        <v>201</v>
       </c>
       <c r="E67" s="41"/>
       <c r="F67" s="41"/>
@@ -4917,7 +4951,7 @@
       <c r="H67" s="41"/>
       <c r="I67" s="30"/>
       <c r="J67" s="25" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
@@ -4969,13 +5003,13 @@
         <v>22</v>
       </c>
       <c r="B69" s="31" t="s">
+        <v>202</v>
+      </c>
+      <c r="C69" s="37" t="s">
         <v>203</v>
       </c>
-      <c r="C69" s="37" t="s">
+      <c r="D69" s="38" t="s">
         <v>204</v>
-      </c>
-      <c r="D69" s="38" t="s">
-        <v>205</v>
       </c>
       <c r="E69" s="41"/>
       <c r="F69" s="41"/>
@@ -5005,13 +5039,13 @@
         <v>22</v>
       </c>
       <c r="B70" s="31" t="s">
+        <v>205</v>
+      </c>
+      <c r="C70" s="37" t="s">
         <v>206</v>
       </c>
-      <c r="C70" s="37" t="s">
+      <c r="D70" s="38" t="s">
         <v>207</v>
-      </c>
-      <c r="D70" s="38" t="s">
-        <v>208</v>
       </c>
       <c r="E70" s="30"/>
       <c r="F70" s="30"/>
@@ -5036,22 +5070,28 @@
       <c r="Y70" s="4"/>
       <c r="Z70" s="4"/>
     </row>
-    <row r="71" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B71" s="5"/>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
-      <c r="E71" s="12"/>
-      <c r="F71" s="12"/>
-      <c r="G71" s="12"/>
-      <c r="H71" s="12"/>
-      <c r="I71" s="12"/>
-      <c r="J71" s="11"/>
-      <c r="K71" s="2"/>
-      <c r="L71" s="2"/>
-      <c r="M71" s="2"/>
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="B71" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="C71" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="D71" s="38" t="s">
+        <v>210</v>
+      </c>
+      <c r="E71" s="30"/>
+      <c r="F71" s="30"/>
+      <c r="G71" s="30"/>
+      <c r="H71" s="30"/>
+      <c r="I71" s="30"/>
+      <c r="J71" s="27"/>
+      <c r="K71" s="4"/>
+      <c r="L71" s="4"/>
+      <c r="M71" s="4"/>
       <c r="N71" s="4"/>
       <c r="O71" s="4"/>
       <c r="P71" s="4"/>
@@ -5067,20 +5107,22 @@
       <c r="Z71" s="4"/>
     </row>
     <row r="72" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="28"/>
-      <c r="B72" s="28"/>
-      <c r="C72" s="28"/>
-      <c r="D72" s="28"/>
-      <c r="E72" s="29"/>
-      <c r="F72" s="29"/>
-      <c r="G72" s="29"/>
-      <c r="H72" s="29"/>
-      <c r="I72" s="29"/>
-      <c r="J72" s="28"/>
+      <c r="A72" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="12"/>
+      <c r="F72" s="12"/>
+      <c r="G72" s="12"/>
+      <c r="H72" s="12"/>
+      <c r="I72" s="12"/>
+      <c r="J72" s="11"/>
       <c r="K72" s="2"/>
       <c r="L72" s="2"/>
       <c r="M72" s="2"/>
-      <c r="N72" s="3"/>
+      <c r="N72" s="4"/>
       <c r="O72" s="4"/>
       <c r="P72" s="4"/>
       <c r="Q72" s="4"/>
@@ -5094,89 +5136,83 @@
       <c r="Y72" s="4"/>
       <c r="Z72" s="4"/>
     </row>
-    <row r="73" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="34"/>
-      <c r="B73" s="34"/>
-      <c r="C73" s="34"/>
-      <c r="D73" s="34"/>
-      <c r="E73" s="35"/>
-      <c r="F73" s="35"/>
-      <c r="G73" s="35"/>
-      <c r="H73" s="35"/>
-      <c r="I73" s="35"/>
-      <c r="J73" s="35"/>
-      <c r="K73" s="36"/>
-      <c r="L73" s="36"/>
-      <c r="M73" s="36"/>
-      <c r="N73" s="36"/>
-      <c r="O73" s="36"/>
-      <c r="P73" s="36"/>
-      <c r="Q73" s="36"/>
-      <c r="R73" s="36"/>
-      <c r="S73" s="36"/>
-      <c r="T73" s="36"/>
-      <c r="U73" s="36"/>
-      <c r="V73" s="36"/>
-      <c r="W73" s="36"/>
-      <c r="X73" s="36"/>
-      <c r="Y73" s="36"/>
-      <c r="Z73" s="36"/>
-    </row>
-    <row r="74" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="11" t="s">
+    <row r="73" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="28"/>
+      <c r="B73" s="28"/>
+      <c r="C73" s="28"/>
+      <c r="D73" s="28"/>
+      <c r="E73" s="29"/>
+      <c r="F73" s="29"/>
+      <c r="G73" s="29"/>
+      <c r="H73" s="29"/>
+      <c r="I73" s="29"/>
+      <c r="J73" s="28"/>
+      <c r="K73" s="2"/>
+      <c r="L73" s="2"/>
+      <c r="M73" s="2"/>
+      <c r="N73" s="3"/>
+      <c r="O73" s="4"/>
+      <c r="P73" s="4"/>
+      <c r="Q73" s="4"/>
+      <c r="R73" s="4"/>
+      <c r="S73" s="4"/>
+      <c r="T73" s="4"/>
+      <c r="U73" s="4"/>
+      <c r="V73" s="4"/>
+      <c r="W73" s="4"/>
+      <c r="X73" s="4"/>
+      <c r="Y73" s="4"/>
+      <c r="Z73" s="4"/>
+    </row>
+    <row r="74" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="34"/>
+      <c r="B74" s="34"/>
+      <c r="C74" s="34"/>
+      <c r="D74" s="34"/>
+      <c r="E74" s="35"/>
+      <c r="F74" s="35"/>
+      <c r="G74" s="35"/>
+      <c r="H74" s="35"/>
+      <c r="I74" s="35"/>
+      <c r="J74" s="35"/>
+      <c r="K74" s="36"/>
+      <c r="L74" s="36"/>
+      <c r="M74" s="36"/>
+      <c r="N74" s="36"/>
+      <c r="O74" s="36"/>
+      <c r="P74" s="36"/>
+      <c r="Q74" s="36"/>
+      <c r="R74" s="36"/>
+      <c r="S74" s="36"/>
+      <c r="T74" s="36"/>
+      <c r="U74" s="36"/>
+      <c r="V74" s="36"/>
+      <c r="W74" s="36"/>
+      <c r="X74" s="36"/>
+      <c r="Y74" s="36"/>
+      <c r="Z74" s="36"/>
+    </row>
+    <row r="75" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B74" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="C74" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="D74" s="11"/>
-      <c r="E74" s="12"/>
-      <c r="F74" s="12"/>
-      <c r="G74" s="12"/>
-      <c r="H74" s="12"/>
-      <c r="I74" s="12"/>
-      <c r="J74" s="11"/>
-      <c r="K74" s="2"/>
-      <c r="L74" s="2"/>
-      <c r="M74" s="2"/>
-      <c r="N74" s="3"/>
-      <c r="O74" s="4"/>
-      <c r="P74" s="4"/>
-      <c r="Q74" s="4"/>
-      <c r="R74" s="4"/>
-      <c r="S74" s="4"/>
-      <c r="T74" s="4"/>
-      <c r="U74" s="4"/>
-      <c r="V74" s="4"/>
-      <c r="W74" s="4"/>
-      <c r="X74" s="4"/>
-      <c r="Y74" s="4"/>
-      <c r="Z74" s="4"/>
-    </row>
-    <row r="75" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B75" s="27" t="s">
+      <c r="B75" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="C75" s="26" t="s">
+      <c r="C75" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="D75" s="27"/>
-      <c r="E75" s="30"/>
-      <c r="F75" s="30"/>
-      <c r="G75" s="30"/>
-      <c r="H75" s="30"/>
-      <c r="I75" s="30"/>
-      <c r="J75" s="27"/>
-      <c r="K75" s="4"/>
-      <c r="L75" s="4"/>
-      <c r="M75" s="4"/>
-      <c r="N75" s="4"/>
+      <c r="D75" s="11"/>
+      <c r="E75" s="12"/>
+      <c r="F75" s="12"/>
+      <c r="G75" s="12"/>
+      <c r="H75" s="12"/>
+      <c r="I75" s="12"/>
+      <c r="J75" s="11"/>
+      <c r="K75" s="2"/>
+      <c r="L75" s="2"/>
+      <c r="M75" s="2"/>
+      <c r="N75" s="3"/>
       <c r="O75" s="4"/>
       <c r="P75" s="4"/>
       <c r="Q75" s="4"/>
@@ -5191,26 +5227,26 @@
       <c r="Z75" s="4"/>
     </row>
     <row r="76" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="31" t="s">
+      <c r="A76" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B76" s="32" t="s">
+      <c r="B76" s="27" t="s">
         <v>213</v>
       </c>
-      <c r="C76" s="45" t="s">
+      <c r="C76" s="26" t="s">
         <v>214</v>
       </c>
-      <c r="D76" s="38"/>
-      <c r="E76" s="39"/>
-      <c r="F76" s="32"/>
+      <c r="D76" s="27"/>
+      <c r="E76" s="30"/>
+      <c r="F76" s="30"/>
       <c r="G76" s="30"/>
       <c r="H76" s="30"/>
-      <c r="I76" s="40"/>
-      <c r="J76" s="25"/>
-      <c r="K76" s="2"/>
-      <c r="L76" s="2"/>
-      <c r="M76" s="2"/>
-      <c r="N76" s="3"/>
+      <c r="I76" s="30"/>
+      <c r="J76" s="27"/>
+      <c r="K76" s="4"/>
+      <c r="L76" s="4"/>
+      <c r="M76" s="4"/>
+      <c r="N76" s="4"/>
       <c r="O76" s="4"/>
       <c r="P76" s="4"/>
       <c r="Q76" s="4"/>
@@ -5225,22 +5261,26 @@
       <c r="Z76" s="4"/>
     </row>
     <row r="77" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B77" s="5"/>
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
-      <c r="E77" s="12"/>
-      <c r="F77" s="12"/>
-      <c r="G77" s="12"/>
-      <c r="H77" s="12"/>
-      <c r="I77" s="12"/>
-      <c r="J77" s="11"/>
+      <c r="A77" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B77" s="32" t="s">
+        <v>215</v>
+      </c>
+      <c r="C77" s="45" t="s">
+        <v>216</v>
+      </c>
+      <c r="D77" s="38"/>
+      <c r="E77" s="39"/>
+      <c r="F77" s="32"/>
+      <c r="G77" s="30"/>
+      <c r="H77" s="30"/>
+      <c r="I77" s="40"/>
+      <c r="J77" s="25"/>
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
       <c r="M77" s="2"/>
-      <c r="N77" s="4"/>
+      <c r="N77" s="3"/>
       <c r="O77" s="4"/>
       <c r="P77" s="4"/>
       <c r="Q77" s="4"/>
@@ -5254,7 +5294,36 @@
       <c r="Y77" s="4"/>
       <c r="Z77" s="4"/>
     </row>
-    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="78" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A78" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B78" s="5"/>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="12"/>
+      <c r="F78" s="12"/>
+      <c r="G78" s="12"/>
+      <c r="H78" s="12"/>
+      <c r="I78" s="12"/>
+      <c r="J78" s="11"/>
+      <c r="K78" s="2"/>
+      <c r="L78" s="2"/>
+      <c r="M78" s="2"/>
+      <c r="N78" s="4"/>
+      <c r="O78" s="4"/>
+      <c r="P78" s="4"/>
+      <c r="Q78" s="4"/>
+      <c r="R78" s="4"/>
+      <c r="S78" s="4"/>
+      <c r="T78" s="4"/>
+      <c r="U78" s="4"/>
+      <c r="V78" s="4"/>
+      <c r="W78" s="4"/>
+      <c r="X78" s="4"/>
+      <c r="Y78" s="4"/>
+      <c r="Z78" s="4"/>
+    </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -5348,7 +5417,7 @@
     <row r="169" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="170" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="171" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="172" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -5368,9 +5437,9 @@
   <dimension ref="A1:Y65536"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A254" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B3" activeCellId="1" sqref="72:77 B3"/>
+      <selection pane="bottomLeft" activeCell="D119" activeCellId="0" sqref="D119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5385,7 +5454,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="46" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B1" s="46" t="s">
         <v>1</v>
@@ -5445,13 +5514,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="42" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B3" s="42" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -5478,13 +5547,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="42" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B4" s="42" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -5544,7 +5613,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D6" s="49"/>
       <c r="E6" s="49"/>
@@ -5577,7 +5646,7 @@
         <v>33</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D7" s="49"/>
       <c r="E7" s="49"/>
@@ -5631,13 +5700,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B9" s="51" t="s">
         <v>41</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -5664,13 +5733,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B10" s="51" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -5697,13 +5766,13 @@
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B11" s="51" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -5730,13 +5799,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B12" s="51" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -5763,13 +5832,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B13" s="51" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -5796,13 +5865,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B14" s="51" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -5829,13 +5898,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="22" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B15" s="51" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -5862,13 +5931,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="22" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -5952,10 +6021,10 @@
         <v>43</v>
       </c>
       <c r="B19" s="51" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -5985,10 +6054,10 @@
         <v>43</v>
       </c>
       <c r="B20" s="51" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
@@ -6018,10 +6087,10 @@
         <v>43</v>
       </c>
       <c r="B21" s="51" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -6051,10 +6120,10 @@
         <v>43</v>
       </c>
       <c r="B22" s="51" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
@@ -6084,10 +6153,10 @@
         <v>43</v>
       </c>
       <c r="B23" s="51" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
@@ -6120,7 +6189,7 @@
         <v>46</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -6150,10 +6219,10 @@
         <v>43</v>
       </c>
       <c r="B25" s="51" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -6183,10 +6252,10 @@
         <v>43</v>
       </c>
       <c r="B26" s="51" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
@@ -6219,7 +6288,7 @@
         <v>21</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -6249,10 +6318,10 @@
         <v>43</v>
       </c>
       <c r="B28" s="51" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -6282,10 +6351,10 @@
         <v>43</v>
       </c>
       <c r="B29" s="51" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -6315,10 +6384,10 @@
         <v>43</v>
       </c>
       <c r="B30" s="51" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -6348,10 +6417,10 @@
         <v>43</v>
       </c>
       <c r="B31" s="51" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
@@ -6381,10 +6450,10 @@
         <v>43</v>
       </c>
       <c r="B32" s="51" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
@@ -6414,10 +6483,10 @@
         <v>43</v>
       </c>
       <c r="B33" s="51" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
@@ -6447,10 +6516,10 @@
         <v>43</v>
       </c>
       <c r="B34" s="51" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
@@ -6480,10 +6549,10 @@
         <v>43</v>
       </c>
       <c r="B35" s="51" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
@@ -6513,10 +6582,10 @@
         <v>43</v>
       </c>
       <c r="B36" s="51" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
@@ -6597,13 +6666,13 @@
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="31" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B39" s="31" t="s">
         <v>91</v>
       </c>
       <c r="C39" s="53" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D39" s="49"/>
       <c r="E39" s="49"/>
@@ -6630,13 +6699,13 @@
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="31" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B40" s="31" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C40" s="53" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="D40" s="49"/>
       <c r="E40" s="49"/>
@@ -6663,13 +6732,13 @@
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="31" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B41" s="31" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C41" s="53" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D41" s="49"/>
       <c r="E41" s="49"/>
@@ -6696,13 +6765,13 @@
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="31" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B42" s="31" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C42" s="53" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="D42" s="49"/>
       <c r="E42" s="49"/>
@@ -6729,13 +6798,13 @@
     </row>
     <row r="43" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="31" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B43" s="31" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="C43" s="53" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="D43" s="49"/>
       <c r="E43" s="49"/>
@@ -6762,13 +6831,13 @@
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="31" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B44" s="31" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C44" s="53" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -6795,13 +6864,13 @@
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="31" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B45" s="31" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C45" s="53" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
@@ -6828,13 +6897,13 @@
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="31" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B46" s="31" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C46" s="53" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
@@ -6861,13 +6930,13 @@
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="31" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B47" s="31" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="C47" s="53" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
@@ -6894,13 +6963,13 @@
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="31" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B48" s="31" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C48" s="53" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
@@ -6927,13 +6996,13 @@
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="31" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B49" s="31" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="C49" s="53" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
@@ -6960,13 +7029,13 @@
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="31" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B50" s="31" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="C50" s="53" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
@@ -6993,13 +7062,13 @@
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="31" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B51" s="31" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="C51" s="53" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
@@ -7026,13 +7095,13 @@
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="31" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B52" s="31" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="C52" s="53" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
@@ -7092,7 +7161,7 @@
         <v>61</v>
       </c>
       <c r="C54" s="54" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
@@ -7122,10 +7191,10 @@
         <v>58</v>
       </c>
       <c r="B55" s="31" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C55" s="54" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
@@ -7182,10 +7251,10 @@
         <v>63</v>
       </c>
       <c r="B57" s="31" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="C57" s="53" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
@@ -7218,7 +7287,7 @@
         <v>66</v>
       </c>
       <c r="C58" s="53" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
@@ -7248,10 +7317,10 @@
         <v>63</v>
       </c>
       <c r="B59" s="31" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="C59" s="53" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
@@ -7281,10 +7350,10 @@
         <v>63</v>
       </c>
       <c r="B60" s="31" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="C60" s="53" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
@@ -7371,7 +7440,7 @@
         <v>96</v>
       </c>
       <c r="C63" s="53" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="D63" s="4"/>
       <c r="E63" s="4"/>
@@ -7401,10 +7470,10 @@
         <v>93</v>
       </c>
       <c r="B64" s="31" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="C64" s="53" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="4"/>
@@ -7434,10 +7503,10 @@
         <v>93</v>
       </c>
       <c r="B65" s="31" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="C65" s="53" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="D65" s="4"/>
       <c r="E65" s="4"/>
@@ -7467,10 +7536,10 @@
         <v>93</v>
       </c>
       <c r="B66" s="31" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="C66" s="53" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="D66" s="4"/>
       <c r="E66" s="4"/>
@@ -7524,13 +7593,13 @@
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="31" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B68" s="31" t="s">
         <v>101</v>
       </c>
       <c r="C68" s="53" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="D68" s="4"/>
       <c r="E68" s="4"/>
@@ -7557,13 +7626,13 @@
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="31" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B69" s="31" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="C69" s="53" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" s="4"/>
@@ -7590,13 +7659,13 @@
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="31" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B70" s="31" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="C70" s="53" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="4"/>
@@ -7623,13 +7692,13 @@
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="31" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B71" s="31" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="C71" s="53" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" s="4"/>
@@ -7656,13 +7725,13 @@
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="31" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B72" s="31" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="C72" s="53" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="D72" s="4"/>
       <c r="E72" s="4"/>
@@ -7689,13 +7758,13 @@
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="31" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B73" s="31" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C73" s="53" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="D73" s="4"/>
       <c r="E73" s="4"/>
@@ -7722,13 +7791,13 @@
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="31" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B74" s="31" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="C74" s="53" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="D74" s="4"/>
       <c r="E74" s="4"/>
@@ -7785,10 +7854,10 @@
         <v>101</v>
       </c>
       <c r="B76" s="40" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C76" s="55" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
@@ -7821,7 +7890,7 @@
         <v>113</v>
       </c>
       <c r="C77" s="55" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="D77" s="4"/>
       <c r="E77" s="4"/>
@@ -7851,10 +7920,10 @@
         <v>101</v>
       </c>
       <c r="B78" s="40" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C78" s="55" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D78" s="4"/>
       <c r="E78" s="4"/>
@@ -7884,10 +7953,10 @@
         <v>101</v>
       </c>
       <c r="B79" s="40" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="C79" s="55" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D79" s="4"/>
       <c r="E79" s="4"/>
@@ -7941,13 +8010,13 @@
     </row>
     <row r="81" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="31" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B81" s="40" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C81" s="55" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D81" s="4"/>
       <c r="E81" s="4"/>
@@ -7974,13 +8043,13 @@
     </row>
     <row r="82" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="31" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B82" s="40" t="s">
         <v>113</v>
       </c>
       <c r="C82" s="55" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="D82" s="4"/>
       <c r="E82" s="4"/>
@@ -8007,13 +8076,13 @@
     </row>
     <row r="83" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="31" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B83" s="40" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C83" s="55" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D83" s="4"/>
       <c r="E83" s="4"/>
@@ -8040,13 +8109,13 @@
     </row>
     <row r="84" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="31" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B84" s="40" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="C84" s="55" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D84" s="4"/>
       <c r="E84" s="4"/>
@@ -8100,13 +8169,13 @@
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="31" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B86" s="40" t="s">
         <v>122</v>
       </c>
       <c r="C86" s="40" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D86" s="4"/>
       <c r="E86" s="4"/>
@@ -8133,13 +8202,13 @@
     </row>
     <row r="87" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="31" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B87" s="40" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="C87" s="55" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="D87" s="4"/>
       <c r="E87" s="4"/>
@@ -8166,13 +8235,13 @@
     </row>
     <row r="88" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="31" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B88" s="40" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C88" s="55" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="D88" s="4"/>
       <c r="E88" s="4"/>
@@ -8199,13 +8268,13 @@
     </row>
     <row r="89" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="31" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B89" s="40" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="C89" s="55" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="D89" s="4"/>
       <c r="E89" s="4"/>
@@ -8232,13 +8301,13 @@
     </row>
     <row r="90" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="31" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B90" s="40" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="C90" s="55" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="D90" s="4"/>
       <c r="E90" s="4"/>
@@ -8292,13 +8361,13 @@
     </row>
     <row r="92" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="31" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B92" s="40" t="s">
         <v>113</v>
       </c>
       <c r="C92" s="55" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="D92" s="4"/>
       <c r="E92" s="4"/>
@@ -8325,13 +8394,13 @@
     </row>
     <row r="93" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="31" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B93" s="40" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C93" s="55" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="D93" s="4"/>
       <c r="E93" s="4"/>
@@ -8358,13 +8427,13 @@
     </row>
     <row r="94" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="31" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B94" s="40" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="C94" s="55" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D94" s="4"/>
       <c r="E94" s="4"/>
@@ -8418,13 +8487,13 @@
     </row>
     <row r="96" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="40" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B96" s="40" t="s">
         <v>131</v>
       </c>
       <c r="C96" s="55" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D96" s="4"/>
       <c r="E96" s="4"/>
@@ -8451,13 +8520,13 @@
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="40" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B97" s="40" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="C97" s="40" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="D97" s="4"/>
       <c r="E97" s="4"/>
@@ -8511,13 +8580,13 @@
     </row>
     <row r="99" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="40" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B99" s="40" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C99" s="55" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D99" s="4"/>
       <c r="E99" s="4"/>
@@ -8544,13 +8613,13 @@
     </row>
     <row r="100" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="40" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B100" s="40" t="s">
         <v>113</v>
       </c>
       <c r="C100" s="55" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="D100" s="4"/>
       <c r="E100" s="4"/>
@@ -8577,13 +8646,13 @@
     </row>
     <row r="101" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="40" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B101" s="40" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="C101" s="55" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D101" s="4"/>
       <c r="E101" s="4"/>
@@ -8664,13 +8733,13 @@
     </row>
     <row r="104" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="43" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B104" s="43" t="s">
         <v>20</v>
       </c>
       <c r="C104" s="53" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="D104" s="4"/>
       <c r="E104" s="4"/>
@@ -8697,13 +8766,13 @@
     </row>
     <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="43" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B105" s="43" t="s">
         <v>108</v>
       </c>
       <c r="C105" s="53" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="D105" s="4"/>
       <c r="E105" s="4"/>
@@ -8757,13 +8826,13 @@
     </row>
     <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B107" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C107" s="53" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="D107" s="4"/>
       <c r="E107" s="4"/>
@@ -8790,13 +8859,13 @@
     </row>
     <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B108" s="31" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="C108" s="53" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="D108" s="4"/>
       <c r="E108" s="4"/>
@@ -8823,13 +8892,13 @@
     </row>
     <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B109" s="31" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="C109" s="53" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="D109" s="4"/>
       <c r="E109" s="4"/>
@@ -8856,13 +8925,13 @@
     </row>
     <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B110" s="31" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="C110" s="53" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="D110" s="4"/>
       <c r="E110" s="4"/>
@@ -8922,7 +8991,7 @@
         <v>152</v>
       </c>
       <c r="C112" s="53" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="D112" s="4"/>
       <c r="E112" s="4"/>
@@ -8952,10 +9021,10 @@
         <v>149</v>
       </c>
       <c r="B113" s="31" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="C113" s="53" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="D113" s="4"/>
       <c r="E113" s="4"/>
@@ -9008,9 +9077,15 @@
       <c r="Y114" s="4"/>
     </row>
     <row r="115" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A115" s="31"/>
-      <c r="B115" s="31"/>
-      <c r="C115" s="31"/>
+      <c r="A115" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="B115" s="31" t="s">
+        <v>360</v>
+      </c>
+      <c r="C115" s="31" t="s">
+        <v>361</v>
+      </c>
       <c r="D115" s="4"/>
       <c r="E115" s="4"/>
       <c r="F115" s="4"/>
@@ -9035,9 +9110,15 @@
       <c r="Y115" s="4"/>
     </row>
     <row r="116" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A116" s="31"/>
-      <c r="B116" s="31"/>
-      <c r="C116" s="31"/>
+      <c r="A116" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="B116" s="31" t="s">
+        <v>362</v>
+      </c>
+      <c r="C116" s="31" t="s">
+        <v>363</v>
+      </c>
       <c r="D116" s="4"/>
       <c r="E116" s="4"/>
       <c r="F116" s="4"/>
@@ -9063,13 +9144,13 @@
     </row>
     <row r="117" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="31" t="s">
-        <v>358</v>
+        <v>209</v>
       </c>
       <c r="B117" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="C117" s="53" t="s">
-        <v>359</v>
+        <v>364</v>
+      </c>
+      <c r="C117" s="31" t="s">
+        <v>365</v>
       </c>
       <c r="D117" s="4"/>
       <c r="E117" s="4"/>
@@ -9096,13 +9177,13 @@
     </row>
     <row r="118" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="31" t="s">
-        <v>358</v>
+        <v>209</v>
       </c>
       <c r="B118" s="31" t="s">
-        <v>360</v>
-      </c>
-      <c r="C118" s="53" t="s">
-        <v>361</v>
+        <v>366</v>
+      </c>
+      <c r="C118" s="31" t="s">
+        <v>367</v>
       </c>
       <c r="D118" s="4"/>
       <c r="E118" s="4"/>
@@ -9129,13 +9210,13 @@
     </row>
     <row r="119" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="31" t="s">
-        <v>358</v>
+        <v>209</v>
       </c>
       <c r="B119" s="31" t="s">
-        <v>362</v>
-      </c>
-      <c r="C119" s="53" t="s">
-        <v>363</v>
+        <v>368</v>
+      </c>
+      <c r="C119" s="31" t="s">
+        <v>369</v>
       </c>
       <c r="D119" s="4"/>
       <c r="E119" s="4"/>
@@ -9187,15 +9268,15 @@
       <c r="X120" s="4"/>
       <c r="Y120" s="4"/>
     </row>
-    <row r="121" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A121" s="40" t="s">
-        <v>364</v>
-      </c>
-      <c r="B121" s="40" t="s">
-        <v>365</v>
-      </c>
-      <c r="C121" s="55" t="s">
-        <v>366</v>
+    <row r="121" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A121" s="31" t="s">
+        <v>370</v>
+      </c>
+      <c r="B121" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="C121" s="53" t="s">
+        <v>371</v>
       </c>
       <c r="D121" s="4"/>
       <c r="E121" s="4"/>
@@ -9220,15 +9301,15 @@
       <c r="X121" s="4"/>
       <c r="Y121" s="4"/>
     </row>
-    <row r="122" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A122" s="40" t="s">
-        <v>364</v>
-      </c>
-      <c r="B122" s="40" t="s">
-        <v>367</v>
-      </c>
-      <c r="C122" s="55" t="s">
-        <v>368</v>
+    <row r="122" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A122" s="31" t="s">
+        <v>370</v>
+      </c>
+      <c r="B122" s="31" t="s">
+        <v>372</v>
+      </c>
+      <c r="C122" s="53" t="s">
+        <v>373</v>
       </c>
       <c r="D122" s="4"/>
       <c r="E122" s="4"/>
@@ -9253,15 +9334,15 @@
       <c r="X122" s="4"/>
       <c r="Y122" s="4"/>
     </row>
-    <row r="123" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A123" s="40" t="s">
-        <v>364</v>
-      </c>
-      <c r="B123" s="40" t="s">
-        <v>369</v>
-      </c>
-      <c r="C123" s="55" t="s">
+    <row r="123" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A123" s="31" t="s">
         <v>370</v>
+      </c>
+      <c r="B123" s="31" t="s">
+        <v>374</v>
+      </c>
+      <c r="C123" s="53" t="s">
+        <v>375</v>
       </c>
       <c r="D123" s="4"/>
       <c r="E123" s="4"/>
@@ -9286,16 +9367,10 @@
       <c r="X123" s="4"/>
       <c r="Y123" s="4"/>
     </row>
-    <row r="124" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A124" s="40" t="s">
-        <v>364</v>
-      </c>
-      <c r="B124" s="40" t="s">
-        <v>371</v>
-      </c>
-      <c r="C124" s="55" t="s">
-        <v>372</v>
-      </c>
+    <row r="124" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A124" s="31"/>
+      <c r="B124" s="31"/>
+      <c r="C124" s="31"/>
       <c r="D124" s="4"/>
       <c r="E124" s="4"/>
       <c r="F124" s="4"/>
@@ -9321,13 +9396,13 @@
     </row>
     <row r="125" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B125" s="40" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="C125" s="55" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="D125" s="4"/>
       <c r="E125" s="4"/>
@@ -9354,13 +9429,13 @@
     </row>
     <row r="126" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B126" s="40" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="C126" s="55" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="D126" s="4"/>
       <c r="E126" s="4"/>
@@ -9387,13 +9462,13 @@
     </row>
     <row r="127" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A127" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B127" s="40" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="C127" s="55" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="D127" s="4"/>
       <c r="E127" s="4"/>
@@ -9420,13 +9495,13 @@
     </row>
     <row r="128" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B128" s="40" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="C128" s="55" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="D128" s="4"/>
       <c r="E128" s="4"/>
@@ -9453,13 +9528,13 @@
     </row>
     <row r="129" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B129" s="40" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="C129" s="55" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="D129" s="4"/>
       <c r="E129" s="4"/>
@@ -9486,13 +9561,13 @@
     </row>
     <row r="130" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B130" s="40" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="C130" s="55" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="D130" s="4"/>
       <c r="E130" s="4"/>
@@ -9519,13 +9594,13 @@
     </row>
     <row r="131" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B131" s="40" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="C131" s="55" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="D131" s="4"/>
       <c r="E131" s="4"/>
@@ -9552,13 +9627,13 @@
     </row>
     <row r="132" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B132" s="40" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="C132" s="55" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="D132" s="4"/>
       <c r="E132" s="4"/>
@@ -9585,13 +9660,13 @@
     </row>
     <row r="133" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B133" s="40" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="C133" s="55" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="D133" s="4"/>
       <c r="E133" s="4"/>
@@ -9618,13 +9693,13 @@
     </row>
     <row r="134" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B134" s="40" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="C134" s="55" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="D134" s="4"/>
       <c r="E134" s="4"/>
@@ -9651,13 +9726,13 @@
     </row>
     <row r="135" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B135" s="40" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="C135" s="55" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="D135" s="4"/>
       <c r="E135" s="4"/>
@@ -9684,13 +9759,13 @@
     </row>
     <row r="136" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B136" s="40" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="C136" s="55" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="D136" s="4"/>
       <c r="E136" s="4"/>
@@ -9717,13 +9792,13 @@
     </row>
     <row r="137" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B137" s="40" t="s">
-        <v>395</v>
+        <v>401</v>
       </c>
       <c r="C137" s="55" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="D137" s="4"/>
       <c r="E137" s="4"/>
@@ -9750,13 +9825,13 @@
     </row>
     <row r="138" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B138" s="40" t="s">
-        <v>397</v>
+        <v>403</v>
       </c>
       <c r="C138" s="55" t="s">
-        <v>398</v>
+        <v>404</v>
       </c>
       <c r="D138" s="4"/>
       <c r="E138" s="4"/>
@@ -9783,13 +9858,13 @@
     </row>
     <row r="139" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A139" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B139" s="40" t="s">
-        <v>399</v>
+        <v>405</v>
       </c>
       <c r="C139" s="55" t="s">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="D139" s="4"/>
       <c r="E139" s="4"/>
@@ -9816,13 +9891,13 @@
     </row>
     <row r="140" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B140" s="40" t="s">
-        <v>401</v>
+        <v>407</v>
       </c>
       <c r="C140" s="55" t="s">
-        <v>402</v>
+        <v>408</v>
       </c>
       <c r="D140" s="4"/>
       <c r="E140" s="4"/>
@@ -9849,13 +9924,13 @@
     </row>
     <row r="141" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A141" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B141" s="40" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="C141" s="55" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="D141" s="4"/>
       <c r="E141" s="4"/>
@@ -9882,13 +9957,13 @@
     </row>
     <row r="142" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A142" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B142" s="40" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="C142" s="55" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="D142" s="4"/>
       <c r="E142" s="4"/>
@@ -9915,13 +9990,13 @@
     </row>
     <row r="143" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A143" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B143" s="40" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="C143" s="55" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="D143" s="4"/>
       <c r="E143" s="4"/>
@@ -9948,13 +10023,13 @@
     </row>
     <row r="144" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B144" s="40" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="C144" s="55" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="D144" s="4"/>
       <c r="E144" s="4"/>
@@ -9981,13 +10056,13 @@
     </row>
     <row r="145" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A145" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B145" s="40" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="C145" s="55" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="D145" s="4"/>
       <c r="E145" s="4"/>
@@ -10014,13 +10089,13 @@
     </row>
     <row r="146" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B146" s="40" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="C146" s="55" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="D146" s="4"/>
       <c r="E146" s="4"/>
@@ -10047,13 +10122,13 @@
     </row>
     <row r="147" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A147" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B147" s="40" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="C147" s="55" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="D147" s="4"/>
       <c r="E147" s="4"/>
@@ -10080,13 +10155,13 @@
     </row>
     <row r="148" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A148" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B148" s="40" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="C148" s="55" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="D148" s="4"/>
       <c r="E148" s="4"/>
@@ -10113,13 +10188,13 @@
     </row>
     <row r="149" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B149" s="40" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="C149" s="55" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="D149" s="4"/>
       <c r="E149" s="4"/>
@@ -10146,13 +10221,13 @@
     </row>
     <row r="150" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B150" s="40" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="C150" s="55" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="D150" s="4"/>
       <c r="E150" s="4"/>
@@ -10179,13 +10254,13 @@
     </row>
     <row r="151" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B151" s="40" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="C151" s="55" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="D151" s="4"/>
       <c r="E151" s="4"/>
@@ -10212,13 +10287,13 @@
     </row>
     <row r="152" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A152" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B152" s="40" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
       <c r="C152" s="55" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="D152" s="4"/>
       <c r="E152" s="4"/>
@@ -10245,13 +10320,13 @@
     </row>
     <row r="153" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A153" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B153" s="40" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="C153" s="55" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="D153" s="4"/>
       <c r="E153" s="4"/>
@@ -10278,13 +10353,13 @@
     </row>
     <row r="154" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A154" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B154" s="40" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="C154" s="55" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="D154" s="4"/>
       <c r="E154" s="4"/>
@@ -10311,13 +10386,13 @@
     </row>
     <row r="155" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A155" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B155" s="40" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="C155" s="55" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="D155" s="4"/>
       <c r="E155" s="4"/>
@@ -10344,13 +10419,13 @@
     </row>
     <row r="156" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A156" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B156" s="40" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="C156" s="55" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
       <c r="D156" s="4"/>
       <c r="E156" s="4"/>
@@ -10377,13 +10452,13 @@
     </row>
     <row r="157" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A157" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B157" s="40" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="C157" s="55" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="D157" s="4"/>
       <c r="E157" s="4"/>
@@ -10410,13 +10485,13 @@
     </row>
     <row r="158" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A158" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B158" s="40" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="C158" s="55" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="D158" s="4"/>
       <c r="E158" s="4"/>
@@ -10443,13 +10518,13 @@
     </row>
     <row r="159" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A159" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B159" s="40" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="C159" s="55" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="D159" s="4"/>
       <c r="E159" s="4"/>
@@ -10476,13 +10551,13 @@
     </row>
     <row r="160" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A160" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B160" s="40" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="C160" s="55" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="D160" s="4"/>
       <c r="E160" s="4"/>
@@ -10509,13 +10584,13 @@
     </row>
     <row r="161" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A161" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B161" s="40" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="C161" s="55" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="D161" s="4"/>
       <c r="E161" s="4"/>
@@ -10542,13 +10617,13 @@
     </row>
     <row r="162" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A162" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B162" s="40" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="C162" s="55" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="D162" s="4"/>
       <c r="E162" s="4"/>
@@ -10575,13 +10650,13 @@
     </row>
     <row r="163" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A163" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B163" s="40" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="C163" s="55" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="D163" s="4"/>
       <c r="E163" s="4"/>
@@ -10608,13 +10683,13 @@
     </row>
     <row r="164" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A164" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B164" s="40" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="C164" s="55" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="D164" s="4"/>
       <c r="E164" s="4"/>
@@ -10641,13 +10716,13 @@
     </row>
     <row r="165" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A165" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B165" s="40" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="C165" s="55" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="D165" s="4"/>
       <c r="E165" s="4"/>
@@ -10674,13 +10749,13 @@
     </row>
     <row r="166" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B166" s="40" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="C166" s="55" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="D166" s="4"/>
       <c r="E166" s="4"/>
@@ -10707,13 +10782,13 @@
     </row>
     <row r="167" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A167" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B167" s="40" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="C167" s="55" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="D167" s="4"/>
       <c r="E167" s="4"/>
@@ -10740,13 +10815,13 @@
     </row>
     <row r="168" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B168" s="40" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="C168" s="55" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="D168" s="4"/>
       <c r="E168" s="4"/>
@@ -10773,13 +10848,13 @@
     </row>
     <row r="169" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A169" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B169" s="40" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="C169" s="55" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="D169" s="4"/>
       <c r="E169" s="4"/>
@@ -10806,13 +10881,13 @@
     </row>
     <row r="170" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A170" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B170" s="40" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="C170" s="55" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="D170" s="4"/>
       <c r="E170" s="4"/>
@@ -10839,13 +10914,13 @@
     </row>
     <row r="171" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A171" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B171" s="40" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="C171" s="55" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="D171" s="4"/>
       <c r="E171" s="4"/>
@@ -10872,13 +10947,13 @@
     </row>
     <row r="172" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A172" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B172" s="40" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="C172" s="55" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="D172" s="4"/>
       <c r="E172" s="4"/>
@@ -10905,13 +10980,13 @@
     </row>
     <row r="173" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A173" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B173" s="40" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="C173" s="55" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
       <c r="D173" s="4"/>
       <c r="E173" s="4"/>
@@ -10938,13 +11013,13 @@
     </row>
     <row r="174" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A174" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B174" s="40" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="C174" s="55" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
       <c r="D174" s="4"/>
       <c r="E174" s="4"/>
@@ -10971,13 +11046,13 @@
     </row>
     <row r="175" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A175" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B175" s="40" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="C175" s="55" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="D175" s="4"/>
       <c r="E175" s="4"/>
@@ -11004,13 +11079,13 @@
     </row>
     <row r="176" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A176" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B176" s="40" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="C176" s="55" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
       <c r="D176" s="4"/>
       <c r="E176" s="4"/>
@@ -11037,13 +11112,13 @@
     </row>
     <row r="177" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A177" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B177" s="40" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
       <c r="C177" s="55" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="D177" s="4"/>
       <c r="E177" s="4"/>
@@ -11070,13 +11145,13 @@
     </row>
     <row r="178" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A178" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B178" s="40" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="C178" s="55" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="D178" s="4"/>
       <c r="E178" s="4"/>
@@ -11103,13 +11178,13 @@
     </row>
     <row r="179" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A179" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B179" s="40" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="C179" s="55" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="D179" s="4"/>
       <c r="E179" s="4"/>
@@ -11136,13 +11211,13 @@
     </row>
     <row r="180" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A180" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B180" s="40" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="C180" s="55" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="D180" s="4"/>
       <c r="E180" s="4"/>
@@ -11169,13 +11244,13 @@
     </row>
     <row r="181" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A181" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B181" s="40" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="C181" s="55" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
       <c r="D181" s="4"/>
       <c r="E181" s="4"/>
@@ -11202,13 +11277,13 @@
     </row>
     <row r="182" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A182" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B182" s="40" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="C182" s="55" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="D182" s="4"/>
       <c r="E182" s="4"/>
@@ -11235,13 +11310,13 @@
     </row>
     <row r="183" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A183" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B183" s="40" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="C183" s="55" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="D183" s="4"/>
       <c r="E183" s="4"/>
@@ -11268,13 +11343,13 @@
     </row>
     <row r="184" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A184" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B184" s="40" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="C184" s="55" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
       <c r="D184" s="4"/>
       <c r="E184" s="4"/>
@@ -11301,13 +11376,13 @@
     </row>
     <row r="185" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A185" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B185" s="40" t="s">
-        <v>491</v>
+        <v>495</v>
       </c>
       <c r="C185" s="55" t="s">
-        <v>492</v>
+        <v>496</v>
       </c>
       <c r="D185" s="4"/>
       <c r="E185" s="4"/>
@@ -11334,13 +11409,13 @@
     </row>
     <row r="186" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A186" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B186" s="40" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
       <c r="C186" s="55" t="s">
-        <v>494</v>
+        <v>498</v>
       </c>
       <c r="D186" s="4"/>
       <c r="E186" s="4"/>
@@ -11367,13 +11442,13 @@
     </row>
     <row r="187" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A187" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B187" s="40" t="s">
-        <v>495</v>
+        <v>499</v>
       </c>
       <c r="C187" s="55" t="s">
-        <v>496</v>
+        <v>500</v>
       </c>
       <c r="D187" s="4"/>
       <c r="E187" s="4"/>
@@ -11400,13 +11475,13 @@
     </row>
     <row r="188" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A188" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B188" s="40" t="s">
-        <v>497</v>
+        <v>501</v>
       </c>
       <c r="C188" s="55" t="s">
-        <v>498</v>
+        <v>502</v>
       </c>
       <c r="D188" s="4"/>
       <c r="E188" s="4"/>
@@ -11433,13 +11508,13 @@
     </row>
     <row r="189" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A189" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B189" s="40" t="s">
-        <v>499</v>
+        <v>503</v>
       </c>
       <c r="C189" s="55" t="s">
-        <v>500</v>
+        <v>504</v>
       </c>
       <c r="D189" s="4"/>
       <c r="E189" s="4"/>
@@ -11466,13 +11541,13 @@
     </row>
     <row r="190" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A190" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B190" s="40" t="s">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="C190" s="55" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
       <c r="D190" s="4"/>
       <c r="E190" s="4"/>
@@ -11499,13 +11574,13 @@
     </row>
     <row r="191" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A191" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B191" s="40" t="s">
-        <v>499</v>
+        <v>507</v>
       </c>
       <c r="C191" s="55" t="s">
-        <v>500</v>
+        <v>508</v>
       </c>
       <c r="D191" s="4"/>
       <c r="E191" s="4"/>
@@ -11532,13 +11607,13 @@
     </row>
     <row r="192" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A192" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B192" s="40" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="C192" s="55" t="s">
-        <v>504</v>
+        <v>510</v>
       </c>
       <c r="D192" s="4"/>
       <c r="E192" s="4"/>
@@ -11565,13 +11640,13 @@
     </row>
     <row r="193" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A193" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B193" s="40" t="s">
-        <v>505</v>
+        <v>511</v>
       </c>
       <c r="C193" s="55" t="s">
-        <v>506</v>
+        <v>512</v>
       </c>
       <c r="D193" s="4"/>
       <c r="E193" s="4"/>
@@ -11598,13 +11673,13 @@
     </row>
     <row r="194" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A194" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B194" s="40" t="s">
-        <v>507</v>
+        <v>513</v>
       </c>
       <c r="C194" s="55" t="s">
-        <v>508</v>
+        <v>514</v>
       </c>
       <c r="D194" s="4"/>
       <c r="E194" s="4"/>
@@ -11631,13 +11706,13 @@
     </row>
     <row r="195" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A195" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B195" s="40" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="C195" s="55" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="D195" s="4"/>
       <c r="E195" s="4"/>
@@ -11664,13 +11739,13 @@
     </row>
     <row r="196" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A196" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B196" s="40" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
       <c r="C196" s="55" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
       <c r="D196" s="4"/>
       <c r="E196" s="4"/>
@@ -11697,13 +11772,13 @@
     </row>
     <row r="197" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A197" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B197" s="40" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="C197" s="55" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
       <c r="D197" s="4"/>
       <c r="E197" s="4"/>
@@ -11730,13 +11805,13 @@
     </row>
     <row r="198" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A198" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B198" s="40" t="s">
-        <v>515</v>
+        <v>519</v>
       </c>
       <c r="C198" s="55" t="s">
-        <v>516</v>
+        <v>520</v>
       </c>
       <c r="D198" s="4"/>
       <c r="E198" s="4"/>
@@ -11763,13 +11838,13 @@
     </row>
     <row r="199" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A199" s="40" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B199" s="40" t="s">
-        <v>517</v>
+        <v>521</v>
       </c>
       <c r="C199" s="55" t="s">
-        <v>518</v>
+        <v>522</v>
       </c>
       <c r="D199" s="4"/>
       <c r="E199" s="4"/>
@@ -11794,10 +11869,16 @@
       <c r="X199" s="4"/>
       <c r="Y199" s="4"/>
     </row>
-    <row r="200" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A200" s="3"/>
-      <c r="B200" s="3"/>
-      <c r="C200" s="3"/>
+    <row r="200" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A200" s="40" t="s">
+        <v>376</v>
+      </c>
+      <c r="B200" s="40" t="s">
+        <v>523</v>
+      </c>
+      <c r="C200" s="55" t="s">
+        <v>524</v>
+      </c>
       <c r="D200" s="4"/>
       <c r="E200" s="4"/>
       <c r="F200" s="4"/>
@@ -11821,15 +11902,15 @@
       <c r="X200" s="4"/>
       <c r="Y200" s="4"/>
     </row>
-    <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="201" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A201" s="40" t="s">
-        <v>519</v>
-      </c>
-      <c r="B201" s="57" t="s">
-        <v>520</v>
-      </c>
-      <c r="C201" s="57" t="s">
-        <v>521</v>
+        <v>376</v>
+      </c>
+      <c r="B201" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="C201" s="55" t="s">
+        <v>526</v>
       </c>
       <c r="D201" s="4"/>
       <c r="E201" s="4"/>
@@ -11854,15 +11935,15 @@
       <c r="X201" s="4"/>
       <c r="Y201" s="4"/>
     </row>
-    <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="202" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A202" s="40" t="s">
-        <v>519</v>
-      </c>
-      <c r="B202" s="57" t="s">
-        <v>522</v>
-      </c>
-      <c r="C202" s="57" t="s">
-        <v>523</v>
+        <v>376</v>
+      </c>
+      <c r="B202" s="40" t="s">
+        <v>527</v>
+      </c>
+      <c r="C202" s="55" t="s">
+        <v>528</v>
       </c>
       <c r="D202" s="4"/>
       <c r="E202" s="4"/>
@@ -11887,15 +11968,15 @@
       <c r="X202" s="4"/>
       <c r="Y202" s="4"/>
     </row>
-    <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="203" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A203" s="40" t="s">
-        <v>519</v>
-      </c>
-      <c r="B203" s="57" t="s">
-        <v>524</v>
-      </c>
-      <c r="C203" s="57" t="s">
-        <v>525</v>
+        <v>376</v>
+      </c>
+      <c r="B203" s="40" t="s">
+        <v>529</v>
+      </c>
+      <c r="C203" s="55" t="s">
+        <v>530</v>
       </c>
       <c r="D203" s="4"/>
       <c r="E203" s="4"/>
@@ -11920,16 +12001,10 @@
       <c r="X203" s="4"/>
       <c r="Y203" s="4"/>
     </row>
-    <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="40" t="s">
-        <v>519</v>
-      </c>
-      <c r="B204" s="57" t="s">
-        <v>526</v>
-      </c>
-      <c r="C204" s="57" t="s">
-        <v>527</v>
-      </c>
+    <row r="204" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A204" s="3"/>
+      <c r="B204" s="3"/>
+      <c r="C204" s="3"/>
       <c r="D204" s="4"/>
       <c r="E204" s="4"/>
       <c r="F204" s="4"/>
@@ -11955,13 +12030,13 @@
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="40" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="B205" s="57" t="s">
-        <v>528</v>
+        <v>532</v>
       </c>
       <c r="C205" s="57" t="s">
-        <v>529</v>
+        <v>533</v>
       </c>
       <c r="D205" s="4"/>
       <c r="E205" s="4"/>
@@ -11988,13 +12063,13 @@
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="40" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="B206" s="57" t="s">
-        <v>530</v>
+        <v>534</v>
       </c>
       <c r="C206" s="57" t="s">
-        <v>531</v>
+        <v>535</v>
       </c>
       <c r="D206" s="4"/>
       <c r="E206" s="4"/>
@@ -12021,13 +12096,13 @@
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="40" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="B207" s="57" t="s">
-        <v>532</v>
+        <v>536</v>
       </c>
       <c r="C207" s="57" t="s">
-        <v>533</v>
+        <v>537</v>
       </c>
       <c r="D207" s="4"/>
       <c r="E207" s="4"/>
@@ -12054,13 +12129,13 @@
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="40" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="B208" s="57" t="s">
-        <v>534</v>
+        <v>538</v>
       </c>
       <c r="C208" s="57" t="s">
-        <v>535</v>
+        <v>539</v>
       </c>
       <c r="D208" s="4"/>
       <c r="E208" s="4"/>
@@ -12087,13 +12162,13 @@
     </row>
     <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="40" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="B209" s="57" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
       <c r="C209" s="57" t="s">
-        <v>537</v>
+        <v>541</v>
       </c>
       <c r="D209" s="4"/>
       <c r="E209" s="4"/>
@@ -12120,13 +12195,13 @@
     </row>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="40" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="B210" s="57" t="s">
-        <v>538</v>
+        <v>542</v>
       </c>
       <c r="C210" s="57" t="s">
-        <v>539</v>
+        <v>543</v>
       </c>
       <c r="D210" s="4"/>
       <c r="E210" s="4"/>
@@ -12153,13 +12228,13 @@
     </row>
     <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="40" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="B211" s="57" t="s">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="C211" s="57" t="s">
-        <v>541</v>
+        <v>545</v>
       </c>
       <c r="D211" s="4"/>
       <c r="E211" s="4"/>
@@ -12186,13 +12261,13 @@
     </row>
     <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="40" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="B212" s="57" t="s">
-        <v>542</v>
+        <v>546</v>
       </c>
       <c r="C212" s="57" t="s">
-        <v>543</v>
+        <v>547</v>
       </c>
       <c r="D212" s="4"/>
       <c r="E212" s="4"/>
@@ -12219,13 +12294,13 @@
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="40" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="B213" s="57" t="s">
-        <v>544</v>
+        <v>548</v>
       </c>
       <c r="C213" s="57" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
       <c r="D213" s="4"/>
       <c r="E213" s="4"/>
@@ -12252,13 +12327,13 @@
     </row>
     <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="40" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="B214" s="57" t="s">
-        <v>546</v>
+        <v>550</v>
       </c>
       <c r="C214" s="57" t="s">
-        <v>547</v>
+        <v>551</v>
       </c>
       <c r="D214" s="4"/>
       <c r="E214" s="4"/>
@@ -12285,13 +12360,13 @@
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="40" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="B215" s="57" t="s">
-        <v>548</v>
+        <v>552</v>
       </c>
       <c r="C215" s="57" t="s">
-        <v>549</v>
+        <v>553</v>
       </c>
       <c r="D215" s="4"/>
       <c r="E215" s="4"/>
@@ -12318,13 +12393,13 @@
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="40" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="B216" s="57" t="s">
-        <v>550</v>
+        <v>554</v>
       </c>
       <c r="C216" s="57" t="s">
-        <v>551</v>
+        <v>555</v>
       </c>
       <c r="D216" s="4"/>
       <c r="E216" s="4"/>
@@ -12351,13 +12426,13 @@
     </row>
     <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="40" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="B217" s="57" t="s">
-        <v>552</v>
+        <v>556</v>
       </c>
       <c r="C217" s="57" t="s">
-        <v>553</v>
+        <v>557</v>
       </c>
       <c r="D217" s="4"/>
       <c r="E217" s="4"/>
@@ -12384,13 +12459,13 @@
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="40" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="B218" s="57" t="s">
-        <v>554</v>
+        <v>558</v>
       </c>
       <c r="C218" s="57" t="s">
-        <v>555</v>
+        <v>559</v>
       </c>
       <c r="D218" s="4"/>
       <c r="E218" s="4"/>
@@ -12417,13 +12492,13 @@
     </row>
     <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="40" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="B219" s="57" t="s">
-        <v>556</v>
+        <v>560</v>
       </c>
       <c r="C219" s="57" t="s">
-        <v>557</v>
+        <v>561</v>
       </c>
       <c r="D219" s="4"/>
       <c r="E219" s="4"/>
@@ -12450,13 +12525,13 @@
     </row>
     <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="40" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="B220" s="57" t="s">
-        <v>558</v>
+        <v>562</v>
       </c>
       <c r="C220" s="57" t="s">
-        <v>559</v>
+        <v>563</v>
       </c>
       <c r="D220" s="4"/>
       <c r="E220" s="4"/>
@@ -12483,13 +12558,13 @@
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="40" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="B221" s="57" t="s">
-        <v>560</v>
+        <v>564</v>
       </c>
       <c r="C221" s="57" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c r="D221" s="4"/>
       <c r="E221" s="4"/>
@@ -12516,13 +12591,13 @@
     </row>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="40" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="B222" s="57" t="s">
-        <v>562</v>
+        <v>566</v>
       </c>
       <c r="C222" s="57" t="s">
-        <v>563</v>
+        <v>567</v>
       </c>
       <c r="D222" s="4"/>
       <c r="E222" s="4"/>
@@ -12549,13 +12624,13 @@
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="40" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="B223" s="57" t="s">
-        <v>564</v>
+        <v>568</v>
       </c>
       <c r="C223" s="57" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="D223" s="4"/>
       <c r="E223" s="4"/>
@@ -12582,13 +12657,13 @@
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="40" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="B224" s="57" t="s">
-        <v>566</v>
+        <v>570</v>
       </c>
       <c r="C224" s="57" t="s">
-        <v>567</v>
+        <v>571</v>
       </c>
       <c r="D224" s="4"/>
       <c r="E224" s="4"/>
@@ -12615,13 +12690,13 @@
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="40" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="B225" s="57" t="s">
-        <v>568</v>
+        <v>572</v>
       </c>
       <c r="C225" s="57" t="s">
-        <v>569</v>
+        <v>573</v>
       </c>
       <c r="D225" s="4"/>
       <c r="E225" s="4"/>
@@ -12648,13 +12723,13 @@
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="40" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="B226" s="57" t="s">
-        <v>570</v>
+        <v>574</v>
       </c>
       <c r="C226" s="57" t="s">
-        <v>571</v>
+        <v>575</v>
       </c>
       <c r="D226" s="4"/>
       <c r="E226" s="4"/>
@@ -12681,13 +12756,13 @@
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="40" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="B227" s="57" t="s">
-        <v>572</v>
+        <v>576</v>
       </c>
       <c r="C227" s="57" t="s">
-        <v>573</v>
+        <v>577</v>
       </c>
       <c r="D227" s="4"/>
       <c r="E227" s="4"/>
@@ -12714,13 +12789,13 @@
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="40" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="B228" s="57" t="s">
-        <v>574</v>
+        <v>578</v>
       </c>
       <c r="C228" s="57" t="s">
-        <v>575</v>
+        <v>579</v>
       </c>
       <c r="D228" s="4"/>
       <c r="E228" s="4"/>
@@ -12747,13 +12822,13 @@
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="40" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="B229" s="57" t="s">
-        <v>576</v>
+        <v>580</v>
       </c>
       <c r="C229" s="57" t="s">
-        <v>577</v>
+        <v>581</v>
       </c>
       <c r="D229" s="4"/>
       <c r="E229" s="4"/>
@@ -12780,13 +12855,13 @@
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="40" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="B230" s="57" t="s">
-        <v>578</v>
+        <v>582</v>
       </c>
       <c r="C230" s="57" t="s">
-        <v>579</v>
+        <v>583</v>
       </c>
       <c r="D230" s="4"/>
       <c r="E230" s="4"/>
@@ -12811,10 +12886,16 @@
       <c r="X230" s="4"/>
       <c r="Y230" s="4"/>
     </row>
-    <row r="231" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A231" s="39"/>
-      <c r="B231" s="39"/>
-      <c r="C231" s="39"/>
+    <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A231" s="40" t="s">
+        <v>531</v>
+      </c>
+      <c r="B231" s="57" t="s">
+        <v>584</v>
+      </c>
+      <c r="C231" s="57" t="s">
+        <v>585</v>
+      </c>
       <c r="D231" s="4"/>
       <c r="E231" s="4"/>
       <c r="F231" s="4"/>
@@ -12838,10 +12919,16 @@
       <c r="X231" s="4"/>
       <c r="Y231" s="4"/>
     </row>
-    <row r="232" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A232" s="39"/>
-      <c r="B232" s="39"/>
-      <c r="C232" s="39"/>
+    <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A232" s="40" t="s">
+        <v>531</v>
+      </c>
+      <c r="B232" s="57" t="s">
+        <v>586</v>
+      </c>
+      <c r="C232" s="57" t="s">
+        <v>587</v>
+      </c>
       <c r="D232" s="4"/>
       <c r="E232" s="4"/>
       <c r="F232" s="4"/>
@@ -12865,15 +12952,15 @@
       <c r="X232" s="4"/>
       <c r="Y232" s="4"/>
     </row>
-    <row r="233" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A233" s="31" t="s">
-        <v>580</v>
-      </c>
-      <c r="B233" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="C233" s="40" t="s">
-        <v>581</v>
+    <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A233" s="40" t="s">
+        <v>531</v>
+      </c>
+      <c r="B233" s="57" t="s">
+        <v>588</v>
+      </c>
+      <c r="C233" s="57" t="s">
+        <v>589</v>
       </c>
       <c r="D233" s="4"/>
       <c r="E233" s="4"/>
@@ -12898,15 +12985,15 @@
       <c r="X233" s="4"/>
       <c r="Y233" s="4"/>
     </row>
-    <row r="234" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A234" s="31" t="s">
-        <v>580</v>
-      </c>
-      <c r="B234" s="32" t="s">
-        <v>582</v>
-      </c>
-      <c r="C234" s="40" t="s">
-        <v>583</v>
+    <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A234" s="40" t="s">
+        <v>531</v>
+      </c>
+      <c r="B234" s="57" t="s">
+        <v>590</v>
+      </c>
+      <c r="C234" s="57" t="s">
+        <v>591</v>
       </c>
       <c r="D234" s="4"/>
       <c r="E234" s="4"/>
@@ -12932,15 +13019,9 @@
       <c r="Y234" s="4"/>
     </row>
     <row r="235" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A235" s="31" t="s">
-        <v>580</v>
-      </c>
-      <c r="B235" s="32" t="s">
-        <v>584</v>
-      </c>
-      <c r="C235" s="40" t="s">
-        <v>585</v>
-      </c>
+      <c r="A235" s="39"/>
+      <c r="B235" s="39"/>
+      <c r="C235" s="39"/>
       <c r="D235" s="4"/>
       <c r="E235" s="4"/>
       <c r="F235" s="4"/>
@@ -12965,15 +13046,9 @@
       <c r="Y235" s="4"/>
     </row>
     <row r="236" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A236" s="31" t="s">
-        <v>580</v>
-      </c>
-      <c r="B236" s="32" t="s">
-        <v>586</v>
-      </c>
-      <c r="C236" s="40" t="s">
-        <v>587</v>
-      </c>
+      <c r="A236" s="39"/>
+      <c r="B236" s="39"/>
+      <c r="C236" s="39"/>
       <c r="D236" s="4"/>
       <c r="E236" s="4"/>
       <c r="F236" s="4"/>
@@ -12999,13 +13074,13 @@
     </row>
     <row r="237" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A237" s="31" t="s">
-        <v>580</v>
+        <v>592</v>
       </c>
       <c r="B237" s="32" t="s">
-        <v>588</v>
+        <v>70</v>
       </c>
       <c r="C237" s="40" t="s">
-        <v>589</v>
+        <v>593</v>
       </c>
       <c r="D237" s="4"/>
       <c r="E237" s="4"/>
@@ -13032,13 +13107,13 @@
     </row>
     <row r="238" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A238" s="31" t="s">
-        <v>580</v>
+        <v>592</v>
       </c>
       <c r="B238" s="32" t="s">
-        <v>590</v>
+        <v>594</v>
       </c>
       <c r="C238" s="40" t="s">
-        <v>591</v>
+        <v>595</v>
       </c>
       <c r="D238" s="4"/>
       <c r="E238" s="4"/>
@@ -13065,13 +13140,13 @@
     </row>
     <row r="239" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A239" s="31" t="s">
-        <v>580</v>
+        <v>592</v>
       </c>
       <c r="B239" s="32" t="s">
-        <v>592</v>
+        <v>596</v>
       </c>
       <c r="C239" s="40" t="s">
-        <v>593</v>
+        <v>597</v>
       </c>
       <c r="D239" s="4"/>
       <c r="E239" s="4"/>
@@ -13098,13 +13173,13 @@
     </row>
     <row r="240" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A240" s="31" t="s">
-        <v>580</v>
+        <v>592</v>
       </c>
       <c r="B240" s="32" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="C240" s="40" t="s">
-        <v>595</v>
+        <v>599</v>
       </c>
       <c r="D240" s="4"/>
       <c r="E240" s="4"/>
@@ -13131,13 +13206,13 @@
     </row>
     <row r="241" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A241" s="31" t="s">
-        <v>580</v>
+        <v>592</v>
       </c>
       <c r="B241" s="32" t="s">
-        <v>596</v>
+        <v>600</v>
       </c>
       <c r="C241" s="40" t="s">
-        <v>597</v>
+        <v>601</v>
       </c>
       <c r="D241" s="4"/>
       <c r="E241" s="4"/>
@@ -13164,13 +13239,13 @@
     </row>
     <row r="242" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A242" s="31" t="s">
-        <v>580</v>
+        <v>592</v>
       </c>
       <c r="B242" s="32" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="C242" s="40" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="D242" s="4"/>
       <c r="E242" s="4"/>
@@ -13197,13 +13272,13 @@
     </row>
     <row r="243" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A243" s="31" t="s">
-        <v>580</v>
+        <v>592</v>
       </c>
       <c r="B243" s="32" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
       <c r="C243" s="40" t="s">
-        <v>601</v>
+        <v>605</v>
       </c>
       <c r="D243" s="4"/>
       <c r="E243" s="4"/>
@@ -13230,13 +13305,13 @@
     </row>
     <row r="244" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A244" s="31" t="s">
-        <v>580</v>
+        <v>592</v>
       </c>
       <c r="B244" s="32" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
       <c r="C244" s="40" t="s">
-        <v>603</v>
+        <v>607</v>
       </c>
       <c r="D244" s="4"/>
       <c r="E244" s="4"/>
@@ -13263,13 +13338,13 @@
     </row>
     <row r="245" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A245" s="31" t="s">
-        <v>580</v>
+        <v>592</v>
       </c>
       <c r="B245" s="32" t="s">
-        <v>604</v>
+        <v>608</v>
       </c>
       <c r="C245" s="40" t="s">
-        <v>605</v>
+        <v>609</v>
       </c>
       <c r="D245" s="4"/>
       <c r="E245" s="4"/>
@@ -13296,13 +13371,13 @@
     </row>
     <row r="246" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A246" s="31" t="s">
-        <v>580</v>
+        <v>592</v>
       </c>
       <c r="B246" s="32" t="s">
-        <v>606</v>
+        <v>610</v>
       </c>
       <c r="C246" s="40" t="s">
-        <v>607</v>
+        <v>611</v>
       </c>
       <c r="D246" s="4"/>
       <c r="E246" s="4"/>
@@ -13329,13 +13404,13 @@
     </row>
     <row r="247" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A247" s="31" t="s">
-        <v>580</v>
+        <v>592</v>
       </c>
       <c r="B247" s="32" t="s">
-        <v>608</v>
+        <v>612</v>
       </c>
       <c r="C247" s="40" t="s">
-        <v>609</v>
+        <v>613</v>
       </c>
       <c r="D247" s="4"/>
       <c r="E247" s="4"/>
@@ -13362,13 +13437,13 @@
     </row>
     <row r="248" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A248" s="31" t="s">
-        <v>580</v>
+        <v>592</v>
       </c>
       <c r="B248" s="32" t="s">
-        <v>610</v>
+        <v>614</v>
       </c>
       <c r="C248" s="40" t="s">
-        <v>611</v>
+        <v>615</v>
       </c>
       <c r="D248" s="4"/>
       <c r="E248" s="4"/>
@@ -13395,13 +13470,13 @@
     </row>
     <row r="249" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A249" s="31" t="s">
-        <v>580</v>
+        <v>592</v>
       </c>
       <c r="B249" s="32" t="s">
-        <v>612</v>
+        <v>616</v>
       </c>
       <c r="C249" s="40" t="s">
-        <v>613</v>
+        <v>617</v>
       </c>
       <c r="D249" s="4"/>
       <c r="E249" s="4"/>
@@ -13428,13 +13503,13 @@
     </row>
     <row r="250" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A250" s="31" t="s">
-        <v>580</v>
+        <v>592</v>
       </c>
       <c r="B250" s="32" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
       <c r="C250" s="40" t="s">
-        <v>615</v>
+        <v>619</v>
       </c>
       <c r="D250" s="4"/>
       <c r="E250" s="4"/>
@@ -13461,13 +13536,13 @@
     </row>
     <row r="251" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A251" s="31" t="s">
-        <v>580</v>
+        <v>592</v>
       </c>
       <c r="B251" s="32" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="C251" s="40" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
       <c r="D251" s="4"/>
       <c r="E251" s="4"/>
@@ -13494,13 +13569,13 @@
     </row>
     <row r="252" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A252" s="31" t="s">
-        <v>580</v>
+        <v>592</v>
       </c>
       <c r="B252" s="32" t="s">
-        <v>618</v>
+        <v>622</v>
       </c>
       <c r="C252" s="40" t="s">
-        <v>619</v>
+        <v>623</v>
       </c>
       <c r="D252" s="4"/>
       <c r="E252" s="4"/>
@@ -13527,13 +13602,13 @@
     </row>
     <row r="253" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A253" s="31" t="s">
-        <v>580</v>
+        <v>592</v>
       </c>
       <c r="B253" s="32" t="s">
-        <v>620</v>
+        <v>624</v>
       </c>
       <c r="C253" s="40" t="s">
-        <v>621</v>
+        <v>625</v>
       </c>
       <c r="D253" s="4"/>
       <c r="E253" s="4"/>
@@ -13560,13 +13635,13 @@
     </row>
     <row r="254" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A254" s="31" t="s">
-        <v>580</v>
+        <v>592</v>
       </c>
       <c r="B254" s="32" t="s">
-        <v>622</v>
+        <v>626</v>
       </c>
       <c r="C254" s="40" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
       <c r="D254" s="4"/>
       <c r="E254" s="4"/>
@@ -13593,13 +13668,13 @@
     </row>
     <row r="255" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A255" s="31" t="s">
-        <v>580</v>
+        <v>592</v>
       </c>
       <c r="B255" s="32" t="s">
-        <v>624</v>
+        <v>628</v>
       </c>
       <c r="C255" s="40" t="s">
-        <v>625</v>
+        <v>629</v>
       </c>
       <c r="D255" s="4"/>
       <c r="E255" s="4"/>
@@ -13626,13 +13701,13 @@
     </row>
     <row r="256" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A256" s="31" t="s">
-        <v>580</v>
+        <v>592</v>
       </c>
       <c r="B256" s="32" t="s">
-        <v>626</v>
+        <v>630</v>
       </c>
       <c r="C256" s="40" t="s">
-        <v>627</v>
+        <v>631</v>
       </c>
       <c r="D256" s="4"/>
       <c r="E256" s="4"/>
@@ -13659,13 +13734,13 @@
     </row>
     <row r="257" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A257" s="31" t="s">
-        <v>580</v>
+        <v>592</v>
       </c>
       <c r="B257" s="32" t="s">
-        <v>628</v>
+        <v>632</v>
       </c>
       <c r="C257" s="40" t="s">
-        <v>629</v>
+        <v>633</v>
       </c>
       <c r="D257" s="4"/>
       <c r="E257" s="4"/>
@@ -13692,13 +13767,13 @@
     </row>
     <row r="258" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A258" s="31" t="s">
-        <v>580</v>
+        <v>592</v>
       </c>
       <c r="B258" s="32" t="s">
-        <v>630</v>
+        <v>634</v>
       </c>
       <c r="C258" s="40" t="s">
-        <v>631</v>
+        <v>635</v>
       </c>
       <c r="D258" s="4"/>
       <c r="E258" s="4"/>
@@ -13725,13 +13800,13 @@
     </row>
     <row r="259" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A259" s="31" t="s">
-        <v>580</v>
+        <v>592</v>
       </c>
       <c r="B259" s="32" t="s">
-        <v>632</v>
+        <v>636</v>
       </c>
       <c r="C259" s="40" t="s">
-        <v>633</v>
+        <v>637</v>
       </c>
       <c r="D259" s="4"/>
       <c r="E259" s="4"/>
@@ -13756,7 +13831,139 @@
       <c r="X259" s="4"/>
       <c r="Y259" s="4"/>
     </row>
-    <row r="1048576" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="260" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A260" s="31" t="s">
+        <v>592</v>
+      </c>
+      <c r="B260" s="32" t="s">
+        <v>638</v>
+      </c>
+      <c r="C260" s="40" t="s">
+        <v>639</v>
+      </c>
+      <c r="D260" s="4"/>
+      <c r="E260" s="4"/>
+      <c r="F260" s="4"/>
+      <c r="G260" s="4"/>
+      <c r="H260" s="4"/>
+      <c r="I260" s="4"/>
+      <c r="J260" s="4"/>
+      <c r="K260" s="4"/>
+      <c r="L260" s="4"/>
+      <c r="M260" s="4"/>
+      <c r="N260" s="4"/>
+      <c r="O260" s="4"/>
+      <c r="P260" s="4"/>
+      <c r="Q260" s="4"/>
+      <c r="R260" s="4"/>
+      <c r="S260" s="4"/>
+      <c r="T260" s="4"/>
+      <c r="U260" s="4"/>
+      <c r="V260" s="4"/>
+      <c r="W260" s="4"/>
+      <c r="X260" s="4"/>
+      <c r="Y260" s="4"/>
+    </row>
+    <row r="261" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A261" s="31" t="s">
+        <v>592</v>
+      </c>
+      <c r="B261" s="32" t="s">
+        <v>640</v>
+      </c>
+      <c r="C261" s="40" t="s">
+        <v>641</v>
+      </c>
+      <c r="D261" s="4"/>
+      <c r="E261" s="4"/>
+      <c r="F261" s="4"/>
+      <c r="G261" s="4"/>
+      <c r="H261" s="4"/>
+      <c r="I261" s="4"/>
+      <c r="J261" s="4"/>
+      <c r="K261" s="4"/>
+      <c r="L261" s="4"/>
+      <c r="M261" s="4"/>
+      <c r="N261" s="4"/>
+      <c r="O261" s="4"/>
+      <c r="P261" s="4"/>
+      <c r="Q261" s="4"/>
+      <c r="R261" s="4"/>
+      <c r="S261" s="4"/>
+      <c r="T261" s="4"/>
+      <c r="U261" s="4"/>
+      <c r="V261" s="4"/>
+      <c r="W261" s="4"/>
+      <c r="X261" s="4"/>
+      <c r="Y261" s="4"/>
+    </row>
+    <row r="262" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A262" s="31" t="s">
+        <v>592</v>
+      </c>
+      <c r="B262" s="32" t="s">
+        <v>642</v>
+      </c>
+      <c r="C262" s="40" t="s">
+        <v>643</v>
+      </c>
+      <c r="D262" s="4"/>
+      <c r="E262" s="4"/>
+      <c r="F262" s="4"/>
+      <c r="G262" s="4"/>
+      <c r="H262" s="4"/>
+      <c r="I262" s="4"/>
+      <c r="J262" s="4"/>
+      <c r="K262" s="4"/>
+      <c r="L262" s="4"/>
+      <c r="M262" s="4"/>
+      <c r="N262" s="4"/>
+      <c r="O262" s="4"/>
+      <c r="P262" s="4"/>
+      <c r="Q262" s="4"/>
+      <c r="R262" s="4"/>
+      <c r="S262" s="4"/>
+      <c r="T262" s="4"/>
+      <c r="U262" s="4"/>
+      <c r="V262" s="4"/>
+      <c r="W262" s="4"/>
+      <c r="X262" s="4"/>
+      <c r="Y262" s="4"/>
+    </row>
+    <row r="263" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A263" s="31" t="s">
+        <v>592</v>
+      </c>
+      <c r="B263" s="32" t="s">
+        <v>644</v>
+      </c>
+      <c r="C263" s="40" t="s">
+        <v>645</v>
+      </c>
+      <c r="D263" s="4"/>
+      <c r="E263" s="4"/>
+      <c r="F263" s="4"/>
+      <c r="G263" s="4"/>
+      <c r="H263" s="4"/>
+      <c r="I263" s="4"/>
+      <c r="J263" s="4"/>
+      <c r="K263" s="4"/>
+      <c r="L263" s="4"/>
+      <c r="M263" s="4"/>
+      <c r="N263" s="4"/>
+      <c r="O263" s="4"/>
+      <c r="P263" s="4"/>
+      <c r="Q263" s="4"/>
+      <c r="R263" s="4"/>
+      <c r="S263" s="4"/>
+      <c r="T263" s="4"/>
+      <c r="U263" s="4"/>
+      <c r="V263" s="4"/>
+      <c r="W263" s="4"/>
+      <c r="X263" s="4"/>
+      <c r="Y263" s="4"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -13776,7 +13983,7 @@
   <dimension ref="A1:Z65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="72:77 C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13791,13 +13998,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="58" t="s">
-        <v>634</v>
+        <v>646</v>
       </c>
       <c r="B1" s="58" t="s">
         <v>15</v>
       </c>
       <c r="C1" s="59" t="s">
-        <v>635</v>
+        <v>647</v>
       </c>
       <c r="D1" s="59"/>
       <c r="E1" s="59"/>
@@ -13825,13 +14032,13 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="61" t="s">
-        <v>636</v>
+        <v>648</v>
       </c>
       <c r="B2" s="61" t="s">
-        <v>636</v>
+        <v>648</v>
       </c>
       <c r="C2" s="59" t="s">
-        <v>637</v>
+        <v>649</v>
       </c>
       <c r="D2" s="59"/>
       <c r="E2" s="59"/>

</xml_diff>